<commit_message>
Ran the May Ensemble run using CRMMS model version 1.2. Added the appropriate date to the mdl file name to indicate the month it was run. The model file is saved in deterministic mode. The May ensemble run was completed with CRMMS ruleset v1.3
Updated output files from the CRMMS ensemble run for May
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -134,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="267">
+  <borders count="827">
     <border>
       <start/>
       <end/>
@@ -408,11 +408,571 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="827">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -754,6 +1314,726 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="505" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="506" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="507" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="508" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="509" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="510" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="511" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="512" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="513" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="514" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="515" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="516" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="517" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="518" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="519" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="520" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="521" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="522" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="523" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="524" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="525" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="526" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="527" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="528" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="529" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="530" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="531" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="532" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="535" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="536" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="537" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="538" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="539" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="544" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="545" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="546" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="551" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="552" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="553" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="558" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="559" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="560" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="565" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="566" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="567" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="568" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="569" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="570" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="571" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="572" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="573" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="574" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="575" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="576" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="577" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="578" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="579" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="580" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="581" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="582" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="583" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="584" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="585" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="586" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="587" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="588" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="589" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="590" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="591" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="592" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="593" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="594" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="595" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="596" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="597" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="598" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="599" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="600" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="601" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="602" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="603" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="604" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="605" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="606" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="607" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="608" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="609" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="610" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="611" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="612" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="613" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="614" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="615" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="616" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="621" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="622" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="623" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="628" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="629" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="630" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="633" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="634" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="635" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="636" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="637" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="638" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="639" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="640" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="641" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="642" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="643" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="644" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="645" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="646" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="647" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="648" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="649" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="650" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="651" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="652" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="653" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="654" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="655" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="656" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="657" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="658" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="659" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="660" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="661" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="662" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="663" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="664" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="665" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="666" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="670" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="671" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="672" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="673" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="674" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="675" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="676" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="677" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="678" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="679" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="680" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="681" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="682" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="683" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="684" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="685" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="686" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="687" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="688" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="689" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="690" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="691" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="692" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="693" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="694" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="695" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="696" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="697" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="698" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="699" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="700" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="701" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="702" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="703" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="704" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="705" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="706" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="707" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="708" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="709" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="710" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="711" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="712" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="713" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="714" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="715" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="716" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="717" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="718" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="719" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="720" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="721" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="722" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="723" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="724" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="725" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="726" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="727" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="728" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="729" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="730" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="731" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="732" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="733" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="734" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="735" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="736" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="737" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="738" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="739" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="740" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="741" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="742" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="743" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="744" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="745" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="746" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="747" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="748" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="749" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="750" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="751" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="752" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="753" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="754" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="755" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="756" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="757" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="758" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="759" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="760" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="761" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="762" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="763" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="764" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="765" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="766" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="767" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="768" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="769" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="770" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="771" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="772" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="773" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="774" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="775" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="776" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="777" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="778" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="779" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="780" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="781" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="782" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="783" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="784" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="785" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="786" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="787" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="788" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="789" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="790" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="791" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="792" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="793" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="794" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="795" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="796" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="797" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="798" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="799" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="800" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="801" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="802" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="803" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="804" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="805" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="806" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="807" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="808" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="809" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="810" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="811" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="812" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="813" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="814" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="815" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="816" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="817" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="818" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="819" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="820" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="821" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="822" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="823" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="824" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="825" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="826" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -850,13 +2130,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -874,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462348.99999981321</v>
@@ -883,13 +2163,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8335583.937196495</v>
+        <v>8299102.2264430393</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -915,13 +2195,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>994796.99999999988</v>
+        <v>1002166.0000000001</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -939,22 +2219,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>944796.99999999988</v>
+        <v>952166.00000000012</v>
       </c>
       <c r="P3">
-        <v>505648.99999963929</v>
+        <v>505648.99999963935</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>6999999.9999978552</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
-        <v>7639775.9999999981</v>
+        <v>7159775.9999978561</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1051,13 +2331,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1075,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -1084,13 +2364,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8375057.5191964954</v>
+        <v>8332735.6644430403</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1116,13 +2396,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -1140,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -1252,13 +2532,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1276,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -1285,13 +2565,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8351818.1051964955</v>
+        <v>8304570.8804430394</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1317,13 +2597,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -1341,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -1453,13 +2733,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1477,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -1486,13 +2766,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8335827.9611964943</v>
+        <v>8301073.2904430386</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1518,13 +2798,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1061359.5000007339</v>
+        <v>1068728.5000007341</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -1542,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1011359.5000007339</v>
+        <v>1018728.500000734</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -1551,13 +2831,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>6999999.9999978552</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
-        <v>7616493.425999999</v>
+        <v>7136493.4259978561</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1654,13 +2934,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1678,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -1687,13 +2967,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8340857.5551964948</v>
+        <v>8314661.2244430399</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1719,13 +2999,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -1743,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -1752,13 +3032,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>6999999.9999978552</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
-        <v>7654589.2299999958</v>
+        <v>7174589.2299978547</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1855,13 +3135,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1879,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -1888,13 +3168,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8361983.3951964956</v>
+        <v>8321839.6724430406</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1920,13 +3200,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -1944,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -2056,13 +3336,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2080,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -2089,13 +3369,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8387287.6091964962</v>
+        <v>8335779.5724430401</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2121,13 +3401,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1281868.9999999066</v>
+        <v>1288433.0999999067</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -2145,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1231868.9999999066</v>
+        <v>1238433.0999999067</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -2257,13 +3537,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2281,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -2290,13 +3570,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8381700.3291964959</v>
+        <v>8318693.9484430412</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2322,13 +3602,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -2346,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -2458,13 +3738,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2482,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -2491,13 +3771,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8318266.0671964958</v>
+        <v>8288755.1744430391</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2523,13 +3803,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -2547,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -2556,13 +3836,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>9499999.9999988247</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
-        <v>7762420.3039999986</v>
+        <v>9782420.3039988279</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -2659,13 +3939,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2683,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -2692,13 +3972,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384671.2931964966</v>
+        <v>8348217.8284430392</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2709,7 +3989,7 @@
         <v>44562</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>61874.99999999853</v>
@@ -2724,16 +4004,16 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>498184.00000000006</v>
+        <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
-        <v>264742</v>
+        <v>204742</v>
       </c>
       <c r="K3">
         <v>17442</v>
@@ -2748,7 +4028,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -2757,16 +4037,16 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>9128518.7319775522</v>
+        <v>7608518.7319999989</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2860,13 +4140,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2884,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -2893,13 +4173,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8340482.727196495</v>
+        <v>8295102.0704430379</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2925,13 +4205,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -2949,7 +4229,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -3061,13 +4341,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3085,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462348.99999981321</v>
@@ -3094,13 +4374,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8357266.9371964959</v>
+        <v>8317416.2264430402</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3126,13 +4406,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>994796.99999999988</v>
+        <v>1002166.0000000001</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -3150,22 +4430,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>944796.99999999988</v>
+        <v>952166.00000000012</v>
       </c>
       <c r="P3">
-        <v>505648.99999963929</v>
+        <v>505648.99999963935</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>9184230.9999775533</v>
+        <v>7664230.9999999981</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -3262,13 +4542,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3286,7 +4566,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -3295,13 +4575,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8297233.9571964955</v>
+        <v>8268648.6064430391</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3327,13 +4607,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -3351,7 +4631,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -3463,13 +4743,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3487,7 +4767,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -3496,13 +4776,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8252488.0371964965</v>
+        <v>8232957.1764430404</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3528,13 +4808,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -3552,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -3664,13 +4944,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3688,7 +4968,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -3697,13 +4977,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8367347.8571964959</v>
+        <v>8326055.6764430385</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3729,13 +5009,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1281868.9999999066</v>
+        <v>1288433.0999999067</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -3753,7 +5033,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1231868.9999999066</v>
+        <v>1238433.0999999067</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -3865,13 +5145,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3889,7 +5169,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -3898,13 +5178,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8379719.6471964959</v>
+        <v>8346447.2564430395</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3930,13 +5210,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -3954,7 +5234,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -4066,13 +5346,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4090,7 +5370,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -4099,13 +5379,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8323673.727196496</v>
+        <v>8284585.3464430394</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4131,13 +5411,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -4155,7 +5435,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -4164,13 +5444,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>6999999.9999978552</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
-        <v>7588713.6499999976</v>
+        <v>7108713.6499978546</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -4267,13 +5547,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4291,7 +5571,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -4300,13 +5580,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8353968.847196497</v>
+        <v>8318731.4464430409</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4332,13 +5612,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1281868.9999999066</v>
+        <v>1288433.0999999067</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -4356,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1231868.9999999066</v>
+        <v>1238433.0999999067</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -4468,13 +5748,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4492,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -4501,13 +5781,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8354211.4971964965</v>
+        <v>8327802.4564430406</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4533,13 +5813,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -4557,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -4669,13 +5949,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4693,7 +5973,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -4702,13 +5982,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8303540.8871964961</v>
+        <v>8279465.5364430416</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4734,13 +6014,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1281868.9999999066</v>
+        <v>1288433.0999999067</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -4758,7 +6038,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1231868.9999999066</v>
+        <v>1238433.0999999067</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -4870,13 +6150,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4894,7 +6174,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -4903,13 +6183,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8353093.2771964958</v>
+        <v>8322168.9764430411</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4935,13 +6215,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -4959,7 +6239,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -5071,13 +6351,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5095,7 +6375,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -5104,13 +6384,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8413606.6671964936</v>
+        <v>8377327.3964430382</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5136,13 +6416,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -5160,7 +6440,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -5272,13 +6552,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5296,7 +6576,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462348.99999981321</v>
@@ -5305,13 +6585,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8388298.9371964959</v>
+        <v>8348324.2264430393</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5337,13 +6617,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>994796.99999999988</v>
+        <v>1002166.0000000001</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -5361,10 +6641,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>944796.99999999988</v>
+        <v>952166.00000000012</v>
       </c>
       <c r="P3">
-        <v>505648.99999963929</v>
+        <v>505648.99999963935</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5473,13 +6753,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5497,7 +6777,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -5506,13 +6786,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8328400.1371964952</v>
+        <v>8302567.3864430403</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5538,13 +6818,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -5562,7 +6842,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -5674,13 +6954,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5698,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -5707,13 +6987,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8376918.0171964969</v>
+        <v>8342401.1464430401</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5739,13 +7019,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -5763,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -5875,13 +7155,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5899,7 +7179,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -5908,13 +7188,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8352340.9071964957</v>
+        <v>8323118.7264430402</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5940,13 +7220,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -5964,7 +7244,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -6076,13 +7356,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6100,7 +7380,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -6109,13 +7389,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8356184.9371964941</v>
+        <v>8321915.2264430402</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6141,13 +7421,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -6165,7 +7445,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -6277,13 +7557,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6301,7 +7581,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -6310,13 +7590,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8399795.7171964962</v>
+        <v>8355514.4064430417</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6342,13 +7622,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -6366,7 +7646,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -6478,13 +7758,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6502,7 +7782,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -6511,13 +7791,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8295279.5071964953</v>
+        <v>8268110.1364430403</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6543,13 +7823,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -6567,7 +7847,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -6679,13 +7959,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6703,7 +7983,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -6712,13 +7992,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8309465.7071964946</v>
+        <v>8289146.9664430404</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6744,13 +8024,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -6768,7 +8048,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -6880,13 +8160,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6904,7 +8184,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -6913,13 +8193,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8339546.4871964948</v>
+        <v>8307910.2564430404</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6945,13 +8225,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>938559.00000000012</v>
+        <v>945949.00000000023</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -6969,7 +8249,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>888559</v>
+        <v>895949.00000000023</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -7081,13 +8361,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7105,7 +8385,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -7114,13 +8394,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8341734.977196495</v>
+        <v>8310262.8364430405</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7146,13 +8426,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1061359.5000007339</v>
+        <v>1068728.5000007341</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -7170,7 +8450,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1011359.5000007339</v>
+        <v>1018728.500000734</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -7282,13 +8562,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7306,7 +8586,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -7315,13 +8595,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8339661.7111964952</v>
+        <v>8308998.5864430396</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7347,13 +8627,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -7371,7 +8651,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -7483,13 +8763,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7507,7 +8787,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -7516,13 +8796,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8372472.6891964953</v>
+        <v>8334046.9564430406</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7548,13 +8828,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -7572,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -7684,13 +8964,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7708,7 +8988,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -7717,13 +8997,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8418181.8431964964</v>
+        <v>8370667.49244304</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7749,13 +9029,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -7773,7 +9053,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -7885,13 +9165,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7909,7 +9189,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -7918,13 +9198,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8423487.4751964957</v>
+        <v>8376853.6764430404</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7950,13 +9230,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -7974,7 +9254,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -8086,13 +9366,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -8110,7 +9390,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -8119,13 +9399,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8343299.4371964959</v>
+        <v>8293547.4684430407</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8151,13 +9431,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1416868.999999813</v>
+        <v>1423433.0999998131</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -8175,7 +9455,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1366868.999999813</v>
+        <v>1373433.0999998131</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>
@@ -8287,13 +9567,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7999.9999999998645</v>
+        <v>7999.9999999998608</v>
       </c>
       <c r="H2">
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1138559</v>
+        <v>1145949.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -8311,7 +9591,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1088559</v>
+        <v>1095949.0000000002</v>
       </c>
       <c r="P2">
         <v>462158.00000000006</v>
@@ -8320,13 +9600,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8230000.0000000009</v>
+        <v>8230000</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8307612.1011964949</v>
+        <v>8262425.6464430392</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8352,13 +9632,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>15999.999999999729</v>
+        <v>15999.999999999725</v>
       </c>
       <c r="H3">
         <v>438184.00000000006</v>
       </c>
       <c r="I3">
-        <v>1038558.999999799</v>
+        <v>1045948.9999997993</v>
       </c>
       <c r="J3">
         <v>204742</v>
@@ -8376,7 +9656,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>988558.99999979895</v>
+        <v>995948.9999997993</v>
       </c>
       <c r="P3">
         <v>454158.00000000029</v>

</xml_diff>